<commit_message>
Created Code for GetSheetIntoObjectArray
</commit_message>
<xml_diff>
--- a/MedicalRecordAutomation/TestData/openemr_data.xlsx
+++ b/MedicalRecordAutomation/TestData/openemr_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Balaji_Dinakaran\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Mine\Company\Thomson Reuters Sep 2024\AutomationFrameworkSolution\MedicalRecordAutomation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7432C40C-3DA5-4EF8-BF86-5F8EDCBDC329}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CE8DCD9-BF46-4796-99F4-42DA763187CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{479C5D84-6BF7-4455-AE24-17D23BDA49DB}"/>
+    <workbookView xWindow="1116" yWindow="1116" windowWidth="17280" windowHeight="8868" activeTab="2" xr2:uid="{479C5D84-6BF7-4455-AE24-17D23BDA49DB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="14">
   <si>
     <t>Username</t>
   </si>
@@ -80,6 +80,9 @@
   </si>
   <si>
     <t>ken123</t>
+  </si>
+  <si>
+    <t>physician</t>
   </si>
 </sst>
 </file>
@@ -475,10 +478,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26EC0BBD-83E7-4C9E-92DC-FBCEBB838AEB}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -521,6 +524,17 @@
         <v>4</v>
       </c>
     </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -530,8 +544,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BEA9B4B-0C3D-4891-9608-2461B194052B}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Updated the TestCaseSource for InvalidLoginTest
</commit_message>
<xml_diff>
--- a/MedicalRecordAutomation/TestData/openemr_data.xlsx
+++ b/MedicalRecordAutomation/TestData/openemr_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Mine\Company\Thomson Reuters Sep 2024\AutomationFrameworkSolution\MedicalRecordAutomation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CE8DCD9-BF46-4796-99F4-42DA763187CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90B3BB19-CFB1-44A1-90CF-DAD8F3BB78D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1116" yWindow="1116" windowWidth="17280" windowHeight="8868" activeTab="2" xr2:uid="{479C5D84-6BF7-4455-AE24-17D23BDA49DB}"/>
   </bookViews>
@@ -481,7 +481,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD1048576"/>
+      <selection activeCell="A3" sqref="A3:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -596,7 +596,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{604DBE59-E4CC-45C5-8A23-AC5BBF78D159}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>

</xml_diff>